<commit_message>
backend ProductoIngrediente, backend Proveedor
</commit_message>
<xml_diff>
--- a/control_templates.xlsx
+++ b/control_templates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\project_bellavista_donut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto Bellavista\bellavista_donuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F017554-953E-468E-B183-8C6F3049F4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826A6F72-F69A-4A15-8556-B1CCCF75E1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
   <si>
     <t>nombre_visual</t>
   </si>
@@ -104,15 +104,55 @@
   </si>
   <si>
     <t>listo</t>
+  </si>
+  <si>
+    <t>crear_prov.html</t>
+  </si>
+  <si>
+    <t>mostrar_prov.html</t>
+  </si>
+  <si>
+    <t>editar_prov.html</t>
+  </si>
+  <si>
+    <t>/crear_prov</t>
+  </si>
+  <si>
+    <t>/mostrar_prov</t>
+  </si>
+  <si>
+    <t>/editar_prov/id</t>
+  </si>
+  <si>
+    <t>comentarios</t>
+  </si>
+  <si>
+    <t>G: no se guarda en Ingrediente</t>
+  </si>
+  <si>
+    <t>G: no aparecen los ingredientes</t>
+  </si>
+  <si>
+    <t>encargado fe_be</t>
+  </si>
+  <si>
+    <t>estado3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -139,13 +179,125 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -159,15 +311,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}" name="Tabla1" displayName="Tabla1" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{69BF39DE-8AAA-4215-B964-99CBD637ECA4}" name="nombre_visual"/>
-    <tableColumn id="2" xr3:uid="{BF9C67B8-5404-48E8-990E-2D8BC8707D08}" name="url"/>
-    <tableColumn id="3" xr3:uid="{0D3BBC70-8921-4D38-891D-17814477F627}" name="encargado fe"/>
-    <tableColumn id="4" xr3:uid="{3BE7A4C8-9472-434C-AFCB-D686166E6469}" name="estado"/>
-    <tableColumn id="5" xr3:uid="{AAEC5321-748D-4D1A-AE75-B6D66ADFBB71}" name="encargado be"/>
-    <tableColumn id="6" xr3:uid="{459E9AFF-B421-4BED-984D-CE781978CBFE}" name="estado2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}" name="Tabla1" displayName="Tabla1" ref="A1:I11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:I11" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{69BF39DE-8AAA-4215-B964-99CBD637ECA4}" name="nombre_visual" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{BF9C67B8-5404-48E8-990E-2D8BC8707D08}" name="url" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{0D3BBC70-8921-4D38-891D-17814477F627}" name="encargado fe" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{3BE7A4C8-9472-434C-AFCB-D686166E6469}" name="estado" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{AAEC5321-748D-4D1A-AE75-B6D66ADFBB71}" name="encargado be" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{459E9AFF-B421-4BED-984D-CE781978CBFE}" name="estado2" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{BBE34195-B3E7-4B7F-A670-80A6E85826BA}" name="comentarios" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D1BE0426-6A42-443E-9558-DBF3E0F1E5AF}" name="encargado fe_be" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{8C34B0C9-23CE-4B2D-81E2-4FA5E6C47FDE}" name="estado3" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -446,177 +601,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="19.85546875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"en proceso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"listo"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"pendiente"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8 F2:F8" xr:uid="{3049B651-5C93-4282-BC2A-2827C38B0180}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11 F2:F11 I2:I11" xr:uid="{3049B651-5C93-4282-BC2A-2827C38B0180}">
       <formula1>tEstado</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
agregando campo img a crear_prod
</commit_message>
<xml_diff>
--- a/control_templates.xlsx
+++ b/control_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto Bellavista\bellavista_donuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92564EE1-40ED-44F0-BE46-1C28526B45B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90BE8EF-CB0F-4815-9811-B2CC48F2921E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>url</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>comentarios</t>
-  </si>
-  <si>
-    <t>G: no se guarda en Ingrediente</t>
   </si>
   <si>
     <t>G: no aparecen los ingredientes</t>
@@ -734,7 +731,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -754,10 +751,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -778,15 +775,15 @@
         <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -816,7 +813,7 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -828,17 +825,15 @@
         <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
@@ -848,7 +843,7 @@
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -860,7 +855,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>19</v>
@@ -873,12 +868,12 @@
         <v>19</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -899,7 +894,7 @@
         <v>22</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>19</v>
@@ -910,7 +905,7 @@
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -940,7 +935,7 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -970,7 +965,7 @@
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -1000,7 +995,7 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>24</v>
@@ -1030,7 +1025,7 @@
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -1060,7 +1055,7 @@
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
finalizando conexión be con crear_prod
</commit_message>
<xml_diff>
--- a/control_templates.xlsx
+++ b/control_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto Bellavista\bellavista_donuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90BE8EF-CB0F-4815-9811-B2CC48F2921E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725F6090-7CE9-439D-A6FA-2B306F4DC5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -731,7 +731,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
@@ -838,7 +838,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
preparando templates para Luis
</commit_message>
<xml_diff>
--- a/control_templates.xlsx
+++ b/control_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto Bellavista\bellavista_donuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725F6090-7CE9-439D-A6FA-2B306F4DC5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5ACFBA6-60F2-49EA-B564-5A5263888B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t>url</t>
   </si>
@@ -167,13 +167,16 @@
   </si>
   <si>
     <t>editar proveedor</t>
+  </si>
+  <si>
+    <t>en corrección</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +187,12 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,7 +233,222 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -422,6 +646,121 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,27 +776,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}" name="Tabla1" displayName="Tabla1" ref="A1:J11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}" name="Tabla1" displayName="Tabla1" ref="A1:J11" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:J11" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{69BF39DE-8AAA-4215-B964-99CBD637ECA4}" name="descripcion" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{1A5507F9-A055-40ED-86E4-034CB57A23F3}" name="nombre_visual2" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{BF9C67B8-5404-48E8-990E-2D8BC8707D08}" name="url" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{0D3BBC70-8921-4D38-891D-17814477F627}" name="encargado fe" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{3BE7A4C8-9472-434C-AFCB-D686166E6469}" name="estado" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{AAEC5321-748D-4D1A-AE75-B6D66ADFBB71}" name="encargado be" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{459E9AFF-B421-4BED-984D-CE781978CBFE}" name="estado2" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{BBE34195-B3E7-4B7F-A670-80A6E85826BA}" name="comentarios" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{D1BE0426-6A42-443E-9558-DBF3E0F1E5AF}" name="encargado fe_be" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{8C34B0C9-23CE-4B2D-81E2-4FA5E6C47FDE}" name="estado3" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{69BF39DE-8AAA-4215-B964-99CBD637ECA4}" name="descripcion" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{1A5507F9-A055-40ED-86E4-034CB57A23F3}" name="nombre_visual2" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{BF9C67B8-5404-48E8-990E-2D8BC8707D08}" name="url" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{0D3BBC70-8921-4D38-891D-17814477F627}" name="encargado fe" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{3BE7A4C8-9472-434C-AFCB-D686166E6469}" name="estado" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{AAEC5321-748D-4D1A-AE75-B6D66ADFBB71}" name="encargado be" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{459E9AFF-B421-4BED-984D-CE781978CBFE}" name="estado2" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{BBE34195-B3E7-4B7F-A670-80A6E85826BA}" name="comentarios" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{D1BE0426-6A42-443E-9558-DBF3E0F1E5AF}" name="encargado fe_be" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{8C34B0C9-23CE-4B2D-81E2-4FA5E6C47FDE}" name="estado3" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B14C201-F907-403A-B061-35B3A9FC8462}" name="estado" displayName="estado" ref="A1:A4" totalsRowShown="0">
-  <autoFilter ref="A1:A4" xr:uid="{1B14C201-F907-403A-B061-35B3A9FC8462}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B14C201-F907-403A-B061-35B3A9FC8462}" name="estado" displayName="estado" ref="A1:A5" totalsRowShown="0">
+  <autoFilter ref="A1:A5" xr:uid="{1B14C201-F907-403A-B061-35B3A9FC8462}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{CD5BD3C4-A4F9-48B1-A2B7-3B7A795B2AD6}" name="estado"/>
   </tableColumns>
@@ -730,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -740,12 +1079,12 @@
     <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="19.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -825,13 +1164,13 @@
         <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3" t="s">
@@ -855,13 +1194,13 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="3" t="s">
@@ -1084,15 +1423,19 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"listo"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"en proceso"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="en corrección">
+      <formula>NOT(ISERROR(SEARCH("en corrección",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1109,11 +1452,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F101365F-2522-4EC0-91A6-94D49F85F3D3}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1133,6 +1481,11 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
models tipo y subtipo, backend editar_prod
</commit_message>
<xml_diff>
--- a/control_templates.xlsx
+++ b/control_templates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto Bellavista\bellavista_donuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5962EFC7-0F55-4D32-A627-9D9611C3CC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F6A670-41B5-4CE7-813E-D1149A22A3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t>url</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>comentarios</t>
-  </si>
-  <si>
-    <t>G: no aparecen los ingredientes</t>
   </si>
   <si>
     <t>encargado fe_be</t>
@@ -239,46 +236,6 @@
   <dxfs count="16">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -444,6 +401,46 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -459,19 +456,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}" name="Tabla1" displayName="Tabla1" ref="A1:J11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}" name="Tabla1" displayName="Tabla1" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J11" xr:uid="{4CFB7E00-C940-414C-BBBA-4BF6635C68EC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{69BF39DE-8AAA-4215-B964-99CBD637ECA4}" name="descripcion" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{1A5507F9-A055-40ED-86E4-034CB57A23F3}" name="nombre_visual2" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{BF9C67B8-5404-48E8-990E-2D8BC8707D08}" name="url" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{0D3BBC70-8921-4D38-891D-17814477F627}" name="encargado fe" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{3BE7A4C8-9472-434C-AFCB-D686166E6469}" name="estado" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{AAEC5321-748D-4D1A-AE75-B6D66ADFBB71}" name="encargado be" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{459E9AFF-B421-4BED-984D-CE781978CBFE}" name="estado2" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{BBE34195-B3E7-4B7F-A670-80A6E85826BA}" name="comentarios" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{D1BE0426-6A42-443E-9558-DBF3E0F1E5AF}" name="encargado fe_be" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{8C34B0C9-23CE-4B2D-81E2-4FA5E6C47FDE}" name="estado3" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{69BF39DE-8AAA-4215-B964-99CBD637ECA4}" name="descripcion" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{1A5507F9-A055-40ED-86E4-034CB57A23F3}" name="nombre_visual2" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{BF9C67B8-5404-48E8-990E-2D8BC8707D08}" name="url" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0D3BBC70-8921-4D38-891D-17814477F627}" name="encargado fe" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{3BE7A4C8-9472-434C-AFCB-D686166E6469}" name="estado" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{AAEC5321-748D-4D1A-AE75-B6D66ADFBB71}" name="encargado be" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{459E9AFF-B421-4BED-984D-CE781978CBFE}" name="estado2" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{BBE34195-B3E7-4B7F-A670-80A6E85826BA}" name="comentarios" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D1BE0426-6A42-443E-9558-DBF3E0F1E5AF}" name="encargado fe_be" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{8C34B0C9-23CE-4B2D-81E2-4FA5E6C47FDE}" name="estado3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -752,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -773,10 +770,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -797,15 +794,15 @@
         <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -835,7 +832,7 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -847,13 +844,13 @@
         <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3" t="s">
@@ -865,7 +862,7 @@
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -877,13 +874,13 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="3" t="s">
@@ -895,7 +892,7 @@
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -913,11 +910,9 @@
         <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="3" t="s">
         <v>19</v>
       </c>
@@ -927,7 +922,7 @@
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -957,7 +952,7 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -987,7 +982,7 @@
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -1008,7 +1003,7 @@
         <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>19</v>
@@ -1019,7 +1014,7 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>24</v>
@@ -1049,7 +1044,7 @@
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -1079,7 +1074,7 @@
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>
@@ -1110,16 +1105,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="en corrección">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="en corrección">
       <formula>NOT(ISERROR(SEARCH("en corrección",A1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"listo"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1170,7 +1165,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando img_not_available y editando agregar en mostrar prod
</commit_message>
<xml_diff>
--- a/control_templates.xlsx
+++ b/control_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto Bellavista\bellavista_donuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F3F490-4F86-4351-B247-D05EB5F40127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384C9F04-5D51-410D-A4B7-90950981F825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
   <si>
     <t>url</t>
   </si>
@@ -170,6 +170,13 @@
   </si>
   <si>
     <t>G: no aparece el proveedor</t>
+  </si>
+  <si>
+    <t>L: js para ingredientes</t>
+  </si>
+  <si>
+    <t>L: mismo tamaño para no_image_available
+G: filtros (activo, inactivo, todos, tipo)</t>
   </si>
 </sst>
 </file>
@@ -750,7 +757,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -762,7 +769,7 @@
     <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="19.85546875" style="1"/>
@@ -852,7 +859,9 @@
       <c r="G3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
@@ -860,7 +869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -882,7 +891,9 @@
       <c r="G4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="I4" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>